<commit_message>
Add another column and problem
</commit_message>
<xml_diff>
--- a/23.04.17/Problems&Solutions.xlsx
+++ b/23.04.17/Problems&Solutions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Problem</t>
   </si>
@@ -43,22 +43,28 @@
     <t>Is it a good question? If it is not then mention the reason</t>
   </si>
   <si>
-    <t>How does a quality of  case study can measure? Is it from length of our report?</t>
-  </si>
-  <si>
-    <t>How should we divide the workload within our members to score a good mark for all?</t>
-  </si>
-  <si>
-    <t>Expectations for the Viva from sir</t>
-  </si>
-  <si>
-    <t>Since case study hasn't a right or wrong answer can we mention so many facts?</t>
-  </si>
-  <si>
-    <t>Is there any option in twitter to measure the reliability of a tweet?</t>
-  </si>
-  <si>
-    <t>If there's nothing for 6th problem, can we suggest to categorize the tweets and appoint an admin for each category?</t>
+    <t>Priority Number of the Problem</t>
+  </si>
+  <si>
+    <t>1. How does a quality of  case study can measure? Is it from length of our report?</t>
+  </si>
+  <si>
+    <t>2. How should we divide the workload within our members to score a good mark for all?</t>
+  </si>
+  <si>
+    <t>4. Since case study hasn't a right or wrong answer can we mention so many facts?</t>
+  </si>
+  <si>
+    <t>3. Expectations for the Viva from sir</t>
+  </si>
+  <si>
+    <t>5. Is there any option in twitter to measure the reliability of a tweet?</t>
+  </si>
+  <si>
+    <t>6. If there's nothing for 6th problem, can we suggest to categorize the tweets and appoint an admin for each category?</t>
+  </si>
+  <si>
+    <t>7. The Analytical Approach or The Problem-Oriented Method suitable for our academic case study?</t>
   </si>
 </sst>
 </file>
@@ -411,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -419,13 +425,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="103" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="104.42578125" customWidth="1"/>
+    <col min="2" max="3" width="52.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,55 +439,63 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with today's discussion
</commit_message>
<xml_diff>
--- a/23.04.17/Problems&Solutions.xlsx
+++ b/23.04.17/Problems&Solutions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Problem</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>8. Is it ok to prove twitter is unreliable for some occasions?</t>
+  </si>
+  <si>
+    <t>didn't ask</t>
+  </si>
+  <si>
+    <t>asked</t>
+  </si>
+  <si>
+    <t>no need to ask</t>
   </si>
 </sst>
 </file>
@@ -423,7 +432,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,40 +479,64 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>